<commit_message>
lista de presençae número de faltas
</commit_message>
<xml_diff>
--- a/build/ensino/2022/12/primeiro-semestre-de-2023/cronograma-mat236.xlsx
+++ b/build/ensino/2022/12/primeiro-semestre-de-2023/cronograma-mat236.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Semanas</t>
   </si>
@@ -100,97 +100,94 @@
     <t xml:space="preserve">Semana 16</t>
   </si>
   <si>
+    <t xml:space="preserve">Regressão linear simples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semana 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segunda prova</t>
+  </si>
+  <si>
+    <t>legenda</t>
+  </si>
+  <si>
+    <t>Feriado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semana de prova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico da semana</t>
+  </si>
+  <si>
+    <t>Programa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantidade de aulas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de aulas sem feriado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação  do curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estatística descritiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total de aula com feriado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probabilidade: probabilidade condicional, regra da multiplicação, teorema da probailidade total e teorema de Bayes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variável aleatória</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalo de confiança - 1 população</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste de Hipóteses - 1 população</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalo de confiança - 2 populações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste de Hipóteses - 2 populações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tópico 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Teste de associação</t>
   </si>
   <si>
-    <t xml:space="preserve">Semana 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regressão linear simples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">semana 18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tópico 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segunda prova</t>
-  </si>
-  <si>
-    <t>legenda</t>
-  </si>
-  <si>
-    <t>Feriado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana de prova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico da semana</t>
-  </si>
-  <si>
-    <t>Programa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade de aulas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de aulas sem feriado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apresentação  do curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estatística descritiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total de aula com feriado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probabilidade: probabilidade condicional, regra da multiplicação, teorema da probailidade total e teorema de Bayes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variável aleatória</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intervalo de confiança - 1 população</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste de Hipóteses - 1 população</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intervalo de confiança - 2 populações</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste de Hipóteses - 2 populações</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tópico 9</t>
   </si>
 </sst>
 </file>
@@ -549,8 +546,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -870,20 +867,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="33" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="34" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="35" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="165" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="35" borderId="9" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="34" borderId="9" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="166" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="33" borderId="10" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="11" numFmtId="166" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -965,8 +958,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="A1:H19">
-  <autoFilter ref="A1:H19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="A1:H18">
+  <autoFilter ref="A1:H18"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Semanas"/>
     <tableColumn id="2" name="Tópico"/>
@@ -1501,16 +1494,16 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1528,16 +1521,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>44990</v>
+        <v>45004</v>
       </c>
       <c r="D2" s="1">
-        <v>44996</v>
+        <v>45010</v>
       </c>
       <c r="E2" s="1">
-        <v>44992</v>
+        <v>45006</v>
       </c>
       <c r="F2" s="1">
-        <v>44994</v>
+        <v>45008</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -1556,19 +1549,19 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C10" si="0">C2+7</f>
-        <v>44997</v>
+        <v>45011</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D10" si="1">D2+7</f>
-        <v>45003</v>
+        <v>45017</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E10" si="2">E2+7</f>
-        <v>44999</v>
+        <v>45013</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F5" si="3">F2+7</f>
-        <v>45001</v>
+        <f t="shared" ref="F3:F10" si="3">F2+7</f>
+        <v>45015</v>
       </c>
       <c r="G3" t="str">
         <f>Programa!$B$3</f>
@@ -1588,19 +1581,19 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>45004</v>
+        <v>45018</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>45010</v>
+        <v>45024</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>45006</v>
+        <v>45020</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="3"/>
-        <v>45008</v>
+        <v>45022</v>
       </c>
       <c r="G4" t="str">
         <f>Programa!$B$4</f>
@@ -1620,19 +1613,19 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>45011</v>
+        <v>45025</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>45017</v>
+        <v>45031</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>45013</v>
+        <v>45027</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="3"/>
-        <v>45015</v>
+        <v>45029</v>
       </c>
       <c r="G5" t="str">
         <f>Programa!$B$4</f>
@@ -1652,19 +1645,19 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>45018</v>
+        <v>45032</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>45024</v>
+        <v>45038</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>45020</v>
+        <v>45034</v>
       </c>
       <c r="F6" s="1">
-        <f>F5+7</f>
-        <v>45022</v>
+        <f t="shared" si="3"/>
+        <v>45036</v>
       </c>
       <c r="G6" t="str">
         <f>Programa!$B$5</f>
@@ -1684,19 +1677,19 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>45025</v>
+        <v>45039</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>45031</v>
+        <v>45045</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>45027</v>
+        <v>45041</v>
       </c>
       <c r="F7" s="1">
-        <f>F6+7</f>
-        <v>45029</v>
+        <f t="shared" si="3"/>
+        <v>45043</v>
       </c>
       <c r="G7" t="str">
         <f>Programa!$B$5</f>
@@ -1716,19 +1709,19 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>45032</v>
+        <v>45046</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>45038</v>
+        <v>45052</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>45034</v>
+        <v>45048</v>
       </c>
       <c r="F8" s="1">
-        <f>F7+7</f>
-        <v>45036</v>
+        <f t="shared" si="3"/>
+        <v>45050</v>
       </c>
       <c r="G8" t="str">
         <f>Programa!$B$6</f>
@@ -1748,19 +1741,19 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>45039</v>
+        <v>45053</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>45045</v>
+        <v>45059</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>45041</v>
+        <v>45055</v>
       </c>
       <c r="F9" s="1">
-        <f>F8+7</f>
-        <v>45043</v>
+        <f t="shared" si="3"/>
+        <v>45057</v>
       </c>
       <c r="G9" t="str">
         <f>Programa!$B$6</f>
@@ -1780,25 +1773,25 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>45046</v>
+        <v>45060</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>45052</v>
+        <v>45066</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>45048</v>
+        <v>45062</v>
       </c>
       <c r="F10" s="1">
-        <f>F9+7</f>
-        <v>45050</v>
+        <f t="shared" si="3"/>
+        <v>45064</v>
       </c>
       <c r="G10" t="str">
         <f>Programa!$B$7</f>
         <v xml:space="preserve">Teste de Hipóteses - 1 população</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1811,20 +1804,20 @@
         <v xml:space="preserve">Tópico 6</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ref="C11:C19" si="4">C10+7</f>
-        <v>45053</v>
+        <f t="shared" ref="C11:C18" si="4">C10+7</f>
+        <v>45067</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:D19" si="5">D10+7</f>
-        <v>45059</v>
+        <f t="shared" ref="D11:D18" si="5">D10+7</f>
+        <v>45073</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E19" si="6">E10+7</f>
-        <v>45055</v>
+        <f t="shared" ref="E11:E18" si="6">E10+7</f>
+        <v>45069</v>
       </c>
       <c r="F11" s="1">
-        <f>F10+7</f>
-        <v>45057</v>
+        <f t="shared" ref="F11:F18" si="7">F10+7</f>
+        <v>45071</v>
       </c>
       <c r="G11" t="str">
         <f>Programa!$B$7</f>
@@ -1844,19 +1837,19 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="4"/>
-        <v>45060</v>
+        <v>45074</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="5"/>
-        <v>45066</v>
+        <v>45080</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="6"/>
-        <v>45062</v>
+        <v>45076</v>
       </c>
       <c r="F12" s="1">
-        <f>F11+7</f>
-        <v>45064</v>
+        <f t="shared" si="7"/>
+        <v>45078</v>
       </c>
       <c r="G12" t="str">
         <f>Programa!$B$8</f>
@@ -1876,19 +1869,19 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="4"/>
-        <v>45067</v>
+        <v>45081</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="5"/>
-        <v>45073</v>
+        <v>45087</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="6"/>
-        <v>45069</v>
-      </c>
-      <c r="F13" s="1">
-        <f>F12+7</f>
-        <v>45071</v>
+        <v>45083</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="7"/>
+        <v>45085</v>
       </c>
       <c r="G13" t="str">
         <f>Programa!$B$8</f>
@@ -1908,19 +1901,19 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="4"/>
-        <v>45074</v>
+        <v>45088</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="5"/>
-        <v>45080</v>
+        <v>45094</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="6"/>
-        <v>45076</v>
+        <v>45090</v>
       </c>
       <c r="F14" s="1">
-        <f>F13+7</f>
-        <v>45078</v>
+        <f t="shared" si="7"/>
+        <v>45092</v>
       </c>
       <c r="G14" t="str">
         <f>Programa!$B$9</f>
@@ -1940,19 +1933,19 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="4"/>
-        <v>45081</v>
+        <v>45095</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="5"/>
-        <v>45087</v>
+        <v>45101</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="6"/>
-        <v>45083</v>
+        <v>45097</v>
       </c>
       <c r="F15" s="4">
-        <f>F14+7</f>
-        <v>45085</v>
+        <f t="shared" si="7"/>
+        <v>45099</v>
       </c>
       <c r="G15" t="str">
         <f>Programa!$B$9</f>
@@ -1972,19 +1965,19 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="4"/>
-        <v>45088</v>
+        <v>45102</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="5"/>
-        <v>45094</v>
+        <v>45108</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="6"/>
-        <v>45090</v>
+        <v>45104</v>
       </c>
       <c r="F16" s="1">
-        <f>F15+7</f>
-        <v>45092</v>
+        <f t="shared" si="7"/>
+        <v>45106</v>
       </c>
       <c r="G16" t="str">
         <f>Programa!$B$10</f>
@@ -2004,19 +1997,19 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="4"/>
-        <v>45095</v>
+        <v>45109</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="5"/>
-        <v>45101</v>
+        <v>45115</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="6"/>
-        <v>45097</v>
+        <v>45111</v>
       </c>
       <c r="F17" s="1">
-        <f>F16+7</f>
-        <v>45099</v>
+        <f t="shared" si="7"/>
+        <v>45113</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -2035,74 +2028,49 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="4"/>
-        <v>45102</v>
+        <v>45116</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="5"/>
-        <v>45108</v>
+        <v>45122</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="6"/>
-        <v>45104</v>
+        <v>45118</v>
       </c>
       <c r="F18" s="1">
-        <f>F17+7</f>
-        <v>45106</v>
+        <f t="shared" si="7"/>
+        <v>45120</v>
       </c>
       <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75">
-      <c r="A19" t="s">
+    </row>
+    <row r="19">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" ht="15.75">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1">
-        <f>C18+7</f>
-        <v>45109</v>
-      </c>
-      <c r="D19" s="1">
-        <f>D18+7</f>
-        <v>45115</v>
-      </c>
-      <c r="E19" s="1">
-        <f>E18+7</f>
-        <v>45111</v>
-      </c>
-      <c r="F19" s="1">
-        <f>F18+7</f>
-        <v>45113</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20"/>
-    <row r="21">
-      <c r="A21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" ht="15.75">
+    </row>
+    <row r="22" ht="14.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2135,27 +2103,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>0.5</v>
       </c>
       <c r="E2">
@@ -2164,109 +2132,109 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="13">
-        <v>3.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>4</v>
       </c>
       <c r="E4">
         <f>SUM(C2:C78)</f>
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C6" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13">
+      <c r="B7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="13" t="s">
+    <row r="8">
+      <c r="A8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="13">
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="13" t="s">
+    <row r="9">
+      <c r="A9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="13">
-        <v>4</v>
+      <c r="C11" s="11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>